<commit_message>
Worked through an Alt in the EDA
</commit_message>
<xml_diff>
--- a/Excel_Challenge_614 - Consecutive Numbers Count.xlsx
+++ b/Excel_Challenge_614 - Consecutive Numbers Count.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713E1597-1BB2-48A1-9926-859566B211F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CC4EEF-9978-405F-B3C8-45D6DAEC9E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>Problem</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>https://www.linkedin.com/feed/update/urn:li:activity:7276808751603421184/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Answer </t>
   </si>
 </sst>
 </file>
@@ -317,6 +320,55 @@
             <a:schemeClr val="tx1"/>
           </a:solidFill>
         </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>267503</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>127857</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="A screenshot of a computer code&#10;&#10;Description automatically generated">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6ABE9D27-1CBE-5BE8-5578-6F937A9ED30C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3474720" y="4023360"/>
+          <a:ext cx="5753903" cy="1590897"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -599,7 +651,9 @@
   <we:alternateReferences>
     <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
   </we:alternateReferences>
-  <we:properties/>
+  <we:properties>
+    <we:property name="projectV0_1-56c6e055-265e-4713-816e-a646dbb708de" value="{&quot;kind&quot;:&quot;AFEJSONBlobNode&quot;,&quot;id&quot;:&quot;{1A1DD0C4-50D6-45C4-9345-1DDA94E7AB42}&quot;}"/>
+  </we:properties>
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
@@ -781,7 +835,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -807,6 +861,12 @@
       <c r="B2">
         <v>2</v>
       </c>
+      <c r="E2">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -822,16 +882,16 @@
         <v>9</v>
       </c>
       <c r="H3" cm="1">
-        <f t="array" ref="H3:H20">_xlfn.SCAN(0, E3:E20&lt;&gt; F3:F20, _xleta.SUM)</f>
-        <v>0</v>
+        <f t="array" ref="H3:H21">_xlfn.SCAN(0, E2:E20&lt;&gt; F2:F20, _xleta.SUM)</f>
+        <v>1</v>
       </c>
       <c r="I3" cm="1">
         <f t="array" ref="I3:I20">_xlfn.BYROW(N(_b=_xlfn.TOROW(_b)),_xleta.SUM)</f>
-        <v>1</v>
-      </c>
-      <c r="J3" t="str" cm="1">
+        <v>2</v>
+      </c>
+      <c r="J3" cm="1">
         <f t="array" ref="J3:J20">IF(_i - 1, _i, "")</f>
-        <v/>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -848,10 +908,10 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4" t="str">
-        <v/>
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -931,10 +991,10 @@
         <v>5</v>
       </c>
       <c r="I8">
-        <v>3</v>
-      </c>
-      <c r="J8">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="J8" t="str">
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -951,7 +1011,7 @@
         <v>1</v>
       </c>
       <c r="H9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I9">
         <v>3</v>
@@ -974,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="H10">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I10">
         <v>3</v>
@@ -997,10 +1057,10 @@
         <v>6</v>
       </c>
       <c r="I11">
-        <v>1</v>
-      </c>
-      <c r="J11" t="str">
-        <v/>
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -1020,10 +1080,10 @@
         <v>7</v>
       </c>
       <c r="I12">
-        <v>2</v>
-      </c>
-      <c r="J12">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J12" t="str">
+        <v/>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1040,7 +1100,7 @@
         <v>4</v>
       </c>
       <c r="H13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -1066,10 +1126,10 @@
         <v>8</v>
       </c>
       <c r="I14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J14">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -1086,7 +1146,7 @@
         <v>5</v>
       </c>
       <c r="H15">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I15">
         <v>4</v>
@@ -1109,7 +1169,7 @@
         <v>5</v>
       </c>
       <c r="H16">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I16">
         <v>4</v>
@@ -1132,7 +1192,7 @@
         <v>5</v>
       </c>
       <c r="H17">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I17">
         <v>4</v>
@@ -1155,10 +1215,10 @@
         <v>9</v>
       </c>
       <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18" t="str">
-        <v/>
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1178,10 +1238,10 @@
         <v>10</v>
       </c>
       <c r="I19">
-        <v>2</v>
-      </c>
-      <c r="J19">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J19" t="str">
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -1198,13 +1258,18 @@
         <v>5</v>
       </c>
       <c r="H20">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I20">
-        <v>2</v>
-      </c>
-      <c r="J20">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="J20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H21">
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -1311,5 +1376,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<AFEJSONBlob xmlns="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0">ewAiAHMAYwBoAGUAbQBhACIAOgAiAGgAdAB0AHAAOgAvAC8AcwBjAGgAZQBtAGEAcwAuAGEAZAB2AGEAbgBjAGUAZABmAG8AcgBtAHUAbABhAGUAbgB2AGkAcgBvAG4AbQBlAG4AdAAuAG8AZgBmAGkAYwBlAGEAcABwAHMALgBsAGkAdgBlAC4AYwBvAG0ALwBhAGYAZQBwAHIAbwBqAGUAYwB0AHMALwAwAC4AMgAiACwAIgBmAGkAbABlAHMAIgA6AFsAewAiAHAAYQB0AGgAIgA6ACIALwBwAHIAbwBqAGUAYwB0AHMALwBXAG8AcgBrAGIAbwBvAGsAIgAsACIAdABlAHgAdAAiADoAIgAvAC8AIAAtAC0ALQAgAFcAbwByAGsAYgBvAG8AawAgAG0AbwBkAHUAbABlACAALQAtAC0AXABuAC8ALwAgAEEAIABmAGkAbABlACAAbwBmACAAbgBhAG0AZQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AcwAgAG8AZgAgAHQAaABlACAAZgBvAHIAbQA6AFwAbgAvAC8AIAAgACAAIABuAGEAbQBlACAAPQAgAGQAZQBmAGkAbgBpAHQAaQBvAG4AOwBcAG4AIgB9AF0ALAAiAHAAcgBvAGoAZQBjAHQATgBhAG0AZQBzACIAOgBbAF0ALAAiAGwAbwBjAGEAbABlACIAOgB7ACIAbABpAHMAdABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHIAbwB3AFMAZQBwAGEAcgBhAHQAbwByACIAOgAiADsAIgAsACIAYwBvAGwAdQBtAG4AUwBlAHAAYQByAGEAdABvAHIAIgA6ACIALAAiACwAIgB0AGgAbwB1AHMAYQBuAGQAcwBTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAsACIALAAiAHQAaABvAHUAcwBhAG4AZABzAFAAbwBzAGkAdABpAG8AbgBzACIAOgBbADMAXQAsACIAZABlAGMAaQBtAGEAbABTAGUAcABhAHIAYQB0AG8AcgAiADoAIgAuACIALAAiAGQAYQB0AGUATwByAGQAZQByACIAOgAiAEQATQBZACIALAAiAGMAdQByAHIAZQBuAGMAeQBTAHkAbQBiAG8AbAAiADoAIgAkACIALAAiAGkAcwBDAHUAcgByAGUAbgBjAHkAUwB5AG0AYgBvAGwATABlAGEAZAAiADoAdAByAHUAZQAsACIAaQBzAEMAdQByAHIAZQBuAGMAeQBTAGUAcABCAHkAUwBwAGEAYwBlACIAOgBmAGEAbABzAGUALAAiAHIAbwB3AEwAZQB0AHQAZQByACIAOgAiAFIAIgAsACIAYwBvAGwAdQBtAG4ATABlAHQAdABlAHIAIgA6ACIAQwAiACwAIgByAGMATABlAGYAdABCAHIAYQBjAGsAZQB0ACIAOgAiAFsAIgAsACIAcgBjAFIAaQBnAGgAdABCAHIAYQBjAGsAZQB0ACIAOgAiAF0AIgAsACIAcwB0AGEAdABlAG0AZQBuAHQAUwBlAHAAYQByAGEAdABvAHIAIgA6ACIAOwAiACwAIgBsAG8AYwBhAGwAZQBOAGEAbQBlACIAOgAiAGUAbgAtAHUAcwAiAH0AfQA=</AFEJSONBlob>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A1DD0C4-50D6-45C4-9345-1DDA94E7AB42}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.advancedformulaenvironment.officeapps.live.com/afejsonblob/1.0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
My EDA is done.
</commit_message>
<xml_diff>
--- a/Excel_Challenge_614 - Consecutive Numbers Count.xlsx
+++ b/Excel_Challenge_614 - Consecutive Numbers Count.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CC4EEF-9978-405F-B3C8-45D6DAEC9E5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6DEA9C-885F-4FA8-A5B8-ED1D4CA581F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -657,6 +657,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -832,10 +835,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D8196C-F681-494E-A98E-963A1FD2EEE7}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:AD41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,7 +846,7 @@
     <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -854,7 +857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>9</v>
       </c>
@@ -868,7 +871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9</v>
       </c>
@@ -893,8 +896,63 @@
         <f t="array" ref="J3:J20">IF(_i - 1, _i, "")</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M3" cm="1">
+        <f t="array" ref="M3:AD3">_xlfn.TOROW(_b)</f>
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>5</v>
+      </c>
+      <c r="S3">
+        <v>6</v>
+      </c>
+      <c r="T3">
+        <v>6</v>
+      </c>
+      <c r="U3">
+        <v>6</v>
+      </c>
+      <c r="V3">
+        <v>7</v>
+      </c>
+      <c r="W3">
+        <v>8</v>
+      </c>
+      <c r="X3">
+        <v>8</v>
+      </c>
+      <c r="Y3">
+        <v>9</v>
+      </c>
+      <c r="Z3">
+        <v>9</v>
+      </c>
+      <c r="AA3">
+        <v>9</v>
+      </c>
+      <c r="AB3">
+        <v>9</v>
+      </c>
+      <c r="AC3">
+        <v>10</v>
+      </c>
+      <c r="AD3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
@@ -913,8 +971,67 @@
       <c r="J4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L4" cm="1">
+        <f t="array" ref="L4:L21">_b</f>
+        <v>1</v>
+      </c>
+      <c r="M4" cm="1">
+        <f t="array" ref="M4:AD21">N(_b=_xlfn.TOROW(_b))</f>
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
+        <v>0</v>
+      </c>
+      <c r="AC4">
+        <v>0</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>7</v>
       </c>
@@ -933,8 +1050,65 @@
       <c r="J5" t="str">
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>8</v>
       </c>
@@ -953,8 +1127,65 @@
       <c r="J6" t="str">
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>1</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>9</v>
       </c>
@@ -973,8 +1204,65 @@
       <c r="J7" t="str">
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
+        <v>0</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -996,8 +1284,65 @@
       <c r="J8" t="str">
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1019,8 +1364,65 @@
       <c r="J9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L9">
+        <v>5</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1042,8 +1444,65 @@
       <c r="J10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>6</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10">
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1062,8 +1521,65 @@
       <c r="J11">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>6</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+      <c r="T11">
+        <v>1</v>
+      </c>
+      <c r="U11">
+        <v>1</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1085,8 +1601,65 @@
       <c r="J12" t="str">
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>6</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>1</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12">
+        <v>0</v>
+      </c>
+      <c r="AD12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1108,8 +1681,65 @@
       <c r="J13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L13">
+        <v>7</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13">
+        <v>0</v>
+      </c>
+      <c r="AD13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1131,8 +1761,65 @@
       <c r="J14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L14">
+        <v>8</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>1</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14">
+        <v>0</v>
+      </c>
+      <c r="AD14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1154,8 +1841,65 @@
       <c r="J15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>8</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>0</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1177,8 +1921,65 @@
       <c r="J16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>9</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>1</v>
+      </c>
+      <c r="Z16">
+        <v>1</v>
+      </c>
+      <c r="AA16">
+        <v>1</v>
+      </c>
+      <c r="AB16">
+        <v>1</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
@@ -1200,8 +2001,65 @@
       <c r="J17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L17">
+        <v>9</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>0</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>1</v>
+      </c>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17">
+        <v>1</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1220,8 +2078,65 @@
       <c r="J18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>9</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>1</v>
+      </c>
+      <c r="AB18">
+        <v>1</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>5</v>
       </c>
@@ -1243,8 +2158,65 @@
       <c r="J19" t="str">
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>9</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>1</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>1</v>
+      </c>
+      <c r="AB19">
+        <v>1</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>5</v>
       </c>
@@ -1266,13 +2238,127 @@
       <c r="J20" t="str">
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>10</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>1</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
       <c r="H21">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>11</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>0</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B23" cm="1">
         <f t="array" ref="B23:B41">_xlfn.LET(
     _xlpm.n,_xlfn._TRO_ALL( A:A),
@@ -1283,47 +2369,47 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B29">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B30">
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B31">
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <v/>
       </c>

</xml_diff>